<commit_message>
Add new script and data
</commit_message>
<xml_diff>
--- a/17.12.21_MTS_PC3/17.12.21_MTS_PC3.xlsx
+++ b/17.12.21_MTS_PC3/17.12.21_MTS_PC3.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="23820" windowHeight="13740"/>
+    <workbookView xWindow="120" yWindow="72" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Фотометрия1" sheetId="1" r:id="rId1"/>
@@ -631,11 +631,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -670,6 +670,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -748,6 +753,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -782,6 +788,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -957,14 +964,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP195"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:42">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1089,7 +1099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:42">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1115,7 +1125,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:42">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1141,7 +1151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:42">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1167,7 +1177,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="6" spans="1:42">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1193,7 +1203,7 @@
         <v>22.49</v>
       </c>
     </row>
-    <row r="7" spans="1:42">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1219,7 +1229,7 @@
         <v>22.88</v>
       </c>
     </row>
-    <row r="8" spans="1:42">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1245,7 +1255,7 @@
         <v>23.49</v>
       </c>
     </row>
-    <row r="9" spans="1:42">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1271,7 +1281,7 @@
         <v>23.88</v>
       </c>
     </row>
-    <row r="10" spans="1:42">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1297,7 +1307,7 @@
         <v>45.98</v>
       </c>
     </row>
-    <row r="11" spans="1:42">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1323,7 +1333,7 @@
         <v>46.37</v>
       </c>
     </row>
-    <row r="12" spans="1:42">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1349,7 +1359,7 @@
         <v>46.97</v>
       </c>
     </row>
-    <row r="13" spans="1:42">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1375,7 +1385,7 @@
         <v>47.37</v>
       </c>
     </row>
-    <row r="14" spans="1:42">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1401,7 +1411,7 @@
         <v>69.459999999999994</v>
       </c>
     </row>
-    <row r="15" spans="1:42">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1427,7 +1437,7 @@
         <v>69.86</v>
       </c>
     </row>
-    <row r="16" spans="1:42">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1453,7 +1463,7 @@
         <v>70.459999999999994</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1479,7 +1489,7 @@
         <v>70.86</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1505,7 +1515,7 @@
         <v>92.95</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1531,7 +1541,7 @@
         <v>93.34</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1557,7 +1567,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1583,7 +1593,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -1609,7 +1619,7 @@
         <v>21.51</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1635,7 +1645,7 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -1661,7 +1671,7 @@
         <v>24.46</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -1687,7 +1697,7 @@
         <v>24.86</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1713,7 +1723,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -1739,7 +1749,7 @@
         <v>45.39</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -1765,7 +1775,7 @@
         <v>47.95</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -1791,7 +1801,7 @@
         <v>48.35</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1817,7 +1827,7 @@
         <v>68.489999999999995</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -1843,7 +1853,7 @@
         <v>68.88</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1869,7 +1879,7 @@
         <v>71.44</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1895,7 +1905,7 @@
         <v>71.83</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -1921,7 +1931,7 @@
         <v>91.97</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -1947,7 +1957,7 @@
         <v>92.37</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -1973,7 +1983,7 @@
         <v>1.95</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -1999,7 +2009,7 @@
         <v>2.35</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -2025,7 +2035,7 @@
         <v>20.53</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -2051,7 +2061,7 @@
         <v>20.93</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -2077,7 +2087,7 @@
         <v>25.44</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -2103,7 +2113,7 @@
         <v>25.83</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -2129,7 +2139,7 @@
         <v>44.02</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -2155,7 +2165,7 @@
         <v>44.42</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -2181,7 +2191,7 @@
         <v>48.93</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>10</v>
       </c>
@@ -2207,7 +2217,7 @@
         <v>49.32</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -2233,7 +2243,7 @@
         <v>67.510000000000005</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -2259,7 +2269,7 @@
         <v>67.900000000000006</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -2285,7 +2295,7 @@
         <v>72.42</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -2311,7 +2321,7 @@
         <v>72.81</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -2337,7 +2347,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -2363,7 +2373,7 @@
         <v>91.39</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -2389,7 +2399,7 @@
         <v>2.93</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -2415,7 +2425,7 @@
         <v>3.32</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -2441,7 +2451,7 @@
         <v>19.559999999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -2467,7 +2477,7 @@
         <v>19.95</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -2493,7 +2503,7 @@
         <v>26.42</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>10</v>
       </c>
@@ -2519,7 +2529,7 @@
         <v>26.81</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>10</v>
       </c>
@@ -2545,7 +2555,7 @@
         <v>43.05</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>10</v>
       </c>
@@ -2571,7 +2581,7 @@
         <v>43.44</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -2597,7 +2607,7 @@
         <v>49.91</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>10</v>
       </c>
@@ -2623,7 +2633,7 @@
         <v>50.3</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -2649,7 +2659,7 @@
         <v>66.53</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>10</v>
       </c>
@@ -2675,7 +2685,7 @@
         <v>66.930000000000007</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>10</v>
       </c>
@@ -2701,7 +2711,7 @@
         <v>73.39</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>10</v>
       </c>
@@ -2727,7 +2737,7 @@
         <v>73.790000000000006</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>10</v>
       </c>
@@ -2753,7 +2763,7 @@
         <v>90.02</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>10</v>
       </c>
@@ -2779,7 +2789,7 @@
         <v>90.41</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>10</v>
       </c>
@@ -2805,7 +2815,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>10</v>
       </c>
@@ -2831,7 +2841,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>10</v>
       </c>
@@ -2857,7 +2867,7 @@
         <v>18.579999999999998</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>10</v>
       </c>
@@ -2883,7 +2893,7 @@
         <v>18.97</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>10</v>
       </c>
@@ -2909,7 +2919,7 @@
         <v>27.39</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>10</v>
       </c>
@@ -2935,7 +2945,7 @@
         <v>27.79</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>10</v>
       </c>
@@ -2961,7 +2971,7 @@
         <v>42.07</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>10</v>
       </c>
@@ -2987,7 +2997,7 @@
         <v>42.46</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>10</v>
       </c>
@@ -3013,7 +3023,7 @@
         <v>50.88</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>10</v>
       </c>
@@ -3039,7 +3049,7 @@
         <v>51.28</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>10</v>
       </c>
@@ -3065,7 +3075,7 @@
         <v>65.56</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>10</v>
       </c>
@@ -3091,7 +3101,7 @@
         <v>65.95</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>10</v>
       </c>
@@ -3117,7 +3127,7 @@
         <v>74.37</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>10</v>
       </c>
@@ -3143,7 +3153,7 @@
         <v>74.760000000000005</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>10</v>
       </c>
@@ -3169,7 +3179,7 @@
         <v>89.04</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>10</v>
       </c>
@@ -3195,7 +3205,7 @@
         <v>89.44</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>10</v>
       </c>
@@ -3221,7 +3231,7 @@
         <v>4.88</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>10</v>
       </c>
@@ -3247,7 +3257,7 @@
         <v>5.28</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>10</v>
       </c>
@@ -3273,7 +3283,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>10</v>
       </c>
@@ -3299,7 +3309,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>10</v>
       </c>
@@ -3325,7 +3335,7 @@
         <v>28.37</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>10</v>
       </c>
@@ -3351,7 +3361,7 @@
         <v>28.76</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>10</v>
       </c>
@@ -3377,7 +3387,7 @@
         <v>41.09</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>10</v>
       </c>
@@ -3403,7 +3413,7 @@
         <v>41.49</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>10</v>
       </c>
@@ -3429,7 +3439,7 @@
         <v>51.86</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>10</v>
       </c>
@@ -3455,7 +3465,7 @@
         <v>52.25</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>10</v>
       </c>
@@ -3481,7 +3491,7 @@
         <v>64.58</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>10</v>
       </c>
@@ -3507,7 +3517,7 @@
         <v>64.97</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>10</v>
       </c>
@@ -3533,7 +3543,7 @@
         <v>75.349999999999994</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>10</v>
       </c>
@@ -3559,7 +3569,7 @@
         <v>75.739999999999995</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>10</v>
       </c>
@@ -3585,7 +3595,7 @@
         <v>88.07</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>10</v>
       </c>
@@ -3611,7 +3621,7 @@
         <v>88.46</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>10</v>
       </c>
@@ -3637,7 +3647,7 @@
         <v>5.86</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>10</v>
       </c>
@@ -3663,7 +3673,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>10</v>
       </c>
@@ -3689,7 +3699,7 @@
         <v>16.63</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>10</v>
       </c>
@@ -3715,7 +3725,7 @@
         <v>17.02</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>10</v>
       </c>
@@ -3741,7 +3751,7 @@
         <v>29.35</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>10</v>
       </c>
@@ -3767,7 +3777,7 @@
         <v>29.74</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>10</v>
       </c>
@@ -3793,7 +3803,7 @@
         <v>40.11</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>10</v>
       </c>
@@ -3819,7 +3829,7 @@
         <v>40.51</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>10</v>
       </c>
@@ -3845,7 +3855,7 @@
         <v>52.84</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>10</v>
       </c>
@@ -3871,7 +3881,7 @@
         <v>53.23</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>10</v>
       </c>
@@ -3897,7 +3907,7 @@
         <v>63.6</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>10</v>
       </c>
@@ -3923,7 +3933,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>10</v>
       </c>
@@ -3949,7 +3959,7 @@
         <v>76.319999999999993</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>10</v>
       </c>
@@ -3975,7 +3985,7 @@
         <v>76.72</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>10</v>
       </c>
@@ -4001,7 +4011,7 @@
         <v>87.09</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>10</v>
       </c>
@@ -4027,7 +4037,7 @@
         <v>87.48</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>10</v>
       </c>
@@ -4053,7 +4063,7 @@
         <v>6.84</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>10</v>
       </c>
@@ -4079,7 +4089,7 @@
         <v>7.23</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>10</v>
       </c>
@@ -4105,7 +4115,7 @@
         <v>15.65</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>10</v>
       </c>
@@ -4131,7 +4141,7 @@
         <v>16.04</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>10</v>
       </c>
@@ -4157,7 +4167,7 @@
         <v>30.32</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>10</v>
       </c>
@@ -4183,7 +4193,7 @@
         <v>30.72</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>10</v>
       </c>
@@ -4209,7 +4219,7 @@
         <v>39.14</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>10</v>
       </c>
@@ -4235,7 +4245,7 @@
         <v>39.53</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>10</v>
       </c>
@@ -4261,7 +4271,7 @@
         <v>53.81</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>10</v>
       </c>
@@ -4287,7 +4297,7 @@
         <v>54.21</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>10</v>
       </c>
@@ -4313,7 +4323,7 @@
         <v>62.63</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>10</v>
       </c>
@@ -4339,7 +4349,7 @@
         <v>63.02</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>10</v>
       </c>
@@ -4365,7 +4375,7 @@
         <v>77.3</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>10</v>
       </c>
@@ -4391,7 +4401,7 @@
         <v>77.69</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>10</v>
       </c>
@@ -4417,7 +4427,7 @@
         <v>86.11</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>10</v>
       </c>
@@ -4443,7 +4453,7 @@
         <v>86.51</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>10</v>
       </c>
@@ -4469,7 +4479,7 @@
         <v>7.81</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>10</v>
       </c>
@@ -4495,7 +4505,7 @@
         <v>8.2100000000000009</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>10</v>
       </c>
@@ -4521,7 +4531,7 @@
         <v>14.67</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>10</v>
       </c>
@@ -4547,7 +4557,7 @@
         <v>15.07</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>10</v>
       </c>
@@ -4573,7 +4583,7 @@
         <v>31.3</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>10</v>
       </c>
@@ -4599,7 +4609,7 @@
         <v>31.69</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>10</v>
       </c>
@@ -4625,7 +4635,7 @@
         <v>38.159999999999997</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>10</v>
       </c>
@@ -4651,7 +4661,7 @@
         <v>38.56</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>10</v>
       </c>
@@ -4677,7 +4687,7 @@
         <v>54.79</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>10</v>
       </c>
@@ -4703,7 +4713,7 @@
         <v>55.18</v>
       </c>
     </row>
-    <row r="142" spans="1:8">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>10</v>
       </c>
@@ -4729,7 +4739,7 @@
         <v>61.65</v>
       </c>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>10</v>
       </c>
@@ -4755,7 +4765,7 @@
         <v>62.04</v>
       </c>
     </row>
-    <row r="144" spans="1:8">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>10</v>
       </c>
@@ -4781,7 +4791,7 @@
         <v>78.28</v>
       </c>
     </row>
-    <row r="145" spans="1:8">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>10</v>
       </c>
@@ -4807,7 +4817,7 @@
         <v>78.67</v>
       </c>
     </row>
-    <row r="146" spans="1:8">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>10</v>
       </c>
@@ -4833,7 +4843,7 @@
         <v>85.14</v>
       </c>
     </row>
-    <row r="147" spans="1:8">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>10</v>
       </c>
@@ -4859,7 +4869,7 @@
         <v>85.53</v>
       </c>
     </row>
-    <row r="148" spans="1:8">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>10</v>
       </c>
@@ -4885,7 +4895,7 @@
         <v>8.7899999999999991</v>
       </c>
     </row>
-    <row r="149" spans="1:8">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>10</v>
       </c>
@@ -4911,7 +4921,7 @@
         <v>9.18</v>
       </c>
     </row>
-    <row r="150" spans="1:8">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>10</v>
       </c>
@@ -4937,7 +4947,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="151" spans="1:8">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>10</v>
       </c>
@@ -4963,7 +4973,7 @@
         <v>14.09</v>
       </c>
     </row>
-    <row r="152" spans="1:8">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>10</v>
       </c>
@@ -4989,7 +4999,7 @@
         <v>32.28</v>
       </c>
     </row>
-    <row r="153" spans="1:8">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>10</v>
       </c>
@@ -5015,7 +5025,7 @@
         <v>32.67</v>
       </c>
     </row>
-    <row r="154" spans="1:8">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>10</v>
       </c>
@@ -5041,7 +5051,7 @@
         <v>37.18</v>
       </c>
     </row>
-    <row r="155" spans="1:8">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>10</v>
       </c>
@@ -5067,7 +5077,7 @@
         <v>37.58</v>
       </c>
     </row>
-    <row r="156" spans="1:8">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>10</v>
       </c>
@@ -5093,7 +5103,7 @@
         <v>55.77</v>
       </c>
     </row>
-    <row r="157" spans="1:8">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>10</v>
       </c>
@@ -5119,7 +5129,7 @@
         <v>56.16</v>
       </c>
     </row>
-    <row r="158" spans="1:8">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>10</v>
       </c>
@@ -5145,7 +5155,7 @@
         <v>60.67</v>
       </c>
     </row>
-    <row r="159" spans="1:8">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>10</v>
       </c>
@@ -5171,7 +5181,7 @@
         <v>61.07</v>
       </c>
     </row>
-    <row r="160" spans="1:8">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>10</v>
       </c>
@@ -5197,7 +5207,7 @@
         <v>79.25</v>
       </c>
     </row>
-    <row r="161" spans="1:8">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>10</v>
       </c>
@@ -5223,7 +5233,7 @@
         <v>79.650000000000006</v>
       </c>
     </row>
-    <row r="162" spans="1:8">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>10</v>
       </c>
@@ -5249,7 +5259,7 @@
         <v>84.16</v>
       </c>
     </row>
-    <row r="163" spans="1:8">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>10</v>
       </c>
@@ -5275,7 +5285,7 @@
         <v>84.55</v>
       </c>
     </row>
-    <row r="164" spans="1:8">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>10</v>
       </c>
@@ -5301,7 +5311,7 @@
         <v>9.77</v>
       </c>
     </row>
-    <row r="165" spans="1:8">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>10</v>
       </c>
@@ -5327,7 +5337,7 @@
         <v>10.16</v>
       </c>
     </row>
-    <row r="166" spans="1:8">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>10</v>
       </c>
@@ -5353,7 +5363,7 @@
         <v>12.72</v>
       </c>
     </row>
-    <row r="167" spans="1:8">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>10</v>
       </c>
@@ -5379,7 +5389,7 @@
         <v>13.11</v>
       </c>
     </row>
-    <row r="168" spans="1:8">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>10</v>
       </c>
@@ -5405,7 +5415,7 @@
         <v>33.25</v>
       </c>
     </row>
-    <row r="169" spans="1:8">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>10</v>
       </c>
@@ -5431,7 +5441,7 @@
         <v>33.65</v>
       </c>
     </row>
-    <row r="170" spans="1:8">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>10</v>
       </c>
@@ -5457,7 +5467,7 @@
         <v>36.21</v>
       </c>
     </row>
-    <row r="171" spans="1:8">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>10</v>
       </c>
@@ -5483,7 +5493,7 @@
         <v>36.6</v>
       </c>
     </row>
-    <row r="172" spans="1:8">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>10</v>
       </c>
@@ -5509,7 +5519,7 @@
         <v>56.74</v>
       </c>
     </row>
-    <row r="173" spans="1:8">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>10</v>
       </c>
@@ -5535,7 +5545,7 @@
         <v>57.14</v>
       </c>
     </row>
-    <row r="174" spans="1:8">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>10</v>
       </c>
@@ -5561,7 +5571,7 @@
         <v>59.7</v>
       </c>
     </row>
-    <row r="175" spans="1:8">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>10</v>
       </c>
@@ -5587,7 +5597,7 @@
         <v>60.09</v>
       </c>
     </row>
-    <row r="176" spans="1:8">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>10</v>
       </c>
@@ -5613,7 +5623,7 @@
         <v>80.23</v>
       </c>
     </row>
-    <row r="177" spans="1:8">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>10</v>
       </c>
@@ -5639,7 +5649,7 @@
         <v>80.62</v>
       </c>
     </row>
-    <row r="178" spans="1:8">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>10</v>
       </c>
@@ -5665,7 +5675,7 @@
         <v>83.18</v>
       </c>
     </row>
-    <row r="179" spans="1:8">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>10</v>
       </c>
@@ -5691,7 +5701,7 @@
         <v>83.58</v>
       </c>
     </row>
-    <row r="180" spans="1:8">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>10</v>
       </c>
@@ -5717,7 +5727,7 @@
         <v>10.74</v>
       </c>
     </row>
-    <row r="181" spans="1:8">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>10</v>
       </c>
@@ -5743,7 +5753,7 @@
         <v>11.14</v>
       </c>
     </row>
-    <row r="182" spans="1:8">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>10</v>
       </c>
@@ -5769,7 +5779,7 @@
         <v>11.74</v>
       </c>
     </row>
-    <row r="183" spans="1:8">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>10</v>
       </c>
@@ -5795,7 +5805,7 @@
         <v>12.14</v>
       </c>
     </row>
-    <row r="184" spans="1:8">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>10</v>
       </c>
@@ -5821,7 +5831,7 @@
         <v>34.229999999999997</v>
       </c>
     </row>
-    <row r="185" spans="1:8">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>10</v>
       </c>
@@ -5847,7 +5857,7 @@
         <v>34.619999999999997</v>
       </c>
     </row>
-    <row r="186" spans="1:8">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>10</v>
       </c>
@@ -5873,7 +5883,7 @@
         <v>35.229999999999997</v>
       </c>
     </row>
-    <row r="187" spans="1:8">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>10</v>
       </c>
@@ -5899,7 +5909,7 @@
         <v>35.619999999999997</v>
       </c>
     </row>
-    <row r="188" spans="1:8">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>10</v>
       </c>
@@ -5925,7 +5935,7 @@
         <v>57.72</v>
       </c>
     </row>
-    <row r="189" spans="1:8">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>10</v>
       </c>
@@ -5951,7 +5961,7 @@
         <v>58.11</v>
       </c>
     </row>
-    <row r="190" spans="1:8">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>10</v>
       </c>
@@ -5977,7 +5987,7 @@
         <v>58.72</v>
       </c>
     </row>
-    <row r="191" spans="1:8">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>10</v>
       </c>
@@ -6003,7 +6013,7 @@
         <v>59.11</v>
       </c>
     </row>
-    <row r="192" spans="1:8">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>10</v>
       </c>
@@ -6029,7 +6039,7 @@
         <v>81.209999999999994</v>
       </c>
     </row>
-    <row r="193" spans="1:8">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>10</v>
       </c>
@@ -6055,7 +6065,7 @@
         <v>81.599999999999994</v>
       </c>
     </row>
-    <row r="194" spans="1:8">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>10</v>
       </c>
@@ -6081,7 +6091,7 @@
         <v>82.2</v>
       </c>
     </row>
-    <row r="195" spans="1:8">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>10</v>
       </c>

</xml_diff>